<commit_message>
Jet2Holidays Automation File Update 1.1
</commit_message>
<xml_diff>
--- a/src/main/java/com/jet2holiday/testdata/Book1.xlsx
+++ b/src/main/java/com/jet2holiday/testdata/Book1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tusha\IdeaProjects\Jet2HolidayAutomation\src\main\java\com\jet2holiday\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D99AAC6-D55A-473D-BA35-DF504460CBF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B597BC90-1BC8-440E-906D-1AFB5CF275A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19F37C3D-65C1-46B0-ADA9-E58E3C0D4028}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{19F37C3D-65C1-46B0-ADA9-E58E3C0D4028}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
+    <sheet name="PassengerDetails" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>tusharjadhav228@gmail.com</t>
   </si>
@@ -52,6 +53,90 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Tushar</t>
+  </si>
+  <si>
+    <t>Jadhav</t>
+  </si>
+  <si>
+    <t>Anjali</t>
+  </si>
+  <si>
+    <t>Patil</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Asalfa</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Mnumber</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>tusharjadhav123@gmail.com</t>
+  </si>
+  <si>
+    <t>CardNumber</t>
+  </si>
+  <si>
+    <t>4111 1111 1111 1111</t>
+  </si>
+  <si>
+    <t>CardName</t>
+  </si>
+  <si>
+    <t>Tushar Jadhav</t>
+  </si>
+  <si>
+    <t>CardMonth</t>
+  </si>
+  <si>
+    <t>CardYear</t>
+  </si>
+  <si>
+    <t>CVV</t>
+  </si>
+  <si>
+    <t>08</t>
   </si>
 </sst>
 </file>
@@ -96,9 +181,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -416,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A4145A3-5603-44FB-BB52-BA7305A62624}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -459,4 +545,198 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBC2647-1098-44DE-A033-8B6E8DBAFF4F}">
+  <dimension ref="A1:Q3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.21875" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="11.109375" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="25.77734375" customWidth="1"/>
+    <col min="13" max="13" width="17.88671875" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="15" max="15" width="11.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>1999</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2">
+        <v>8745963287</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2">
+        <v>2026</v>
+      </c>
+      <c r="Q2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3">
+        <v>17</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>2001</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3">
+        <v>8745963287</v>
+      </c>
+      <c r="L3" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3">
+        <v>2028</v>
+      </c>
+      <c r="Q3">
+        <v>456</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{7FF890B0-1B98-4227-A339-D36D57434099}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{373FC10B-1472-49B2-A866-A77429548797}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{8F0E56EC-ABAC-4D52-AA91-06135A418847}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{289E36E3-63E8-40EC-83B2-F4477806E2A8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Jet2Holidays Automation File Update 2.1
</commit_message>
<xml_diff>
--- a/src/main/java/com/jet2holiday/testdata/Book1.xlsx
+++ b/src/main/java/com/jet2holiday/testdata/Book1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tusha\IdeaProjects\Jet2HolidayAutomation\src\main\java\com\jet2holiday\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B597BC90-1BC8-440E-906D-1AFB5CF275A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65305CCD-787F-4154-8219-3F726839EA0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{19F37C3D-65C1-46B0-ADA9-E58E3C0D4028}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginDetails" sheetId="1" r:id="rId1"/>
-    <sheet name="PassengerDetails" sheetId="2" r:id="rId2"/>
+    <sheet name="UserDetails" sheetId="3" r:id="rId2"/>
+    <sheet name="PassengerDetails" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="34">
   <si>
     <t>tusharjadhav228@gmail.com</t>
   </si>
@@ -503,7 +504,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,21 +539,93 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{B00308EE-DE37-4CAA-9E58-816B8B257B16}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{5BB4414B-E4D4-45FB-9BB7-FA5A3E3FABFC}"/>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{5BB4414B-E4D4-45FB-9BB7-FA5A3E3FABFC}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{ED299C87-73C2-4A49-AC07-1AA42F420751}"/>
     <hyperlink ref="B2" r:id="rId3" xr:uid="{4E311DA9-AF46-4ED9-99C1-9337458EEA6F}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{ED299C87-73C2-4A49-AC07-1AA42F420751}"/>
+    <hyperlink ref="A2" r:id="rId4" xr:uid="{B00308EE-DE37-4CAA-9E58-816B8B257B16}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D16FCF7-B307-4FAC-A63D-784C878C6450}">
+  <dimension ref="A2:Q2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2">
+        <v>8</v>
+      </c>
+      <c r="G2">
+        <v>1999</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2">
+        <v>8745963287</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="P2">
+        <v>2026</v>
+      </c>
+      <c r="Q2">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{884CDDDB-E80B-4219-AE79-AB1E6FF164F6}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{6D772E3E-8EF6-4618-A594-420289DE4F30}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EBC2647-1098-44DE-A033-8B6E8DBAFF4F}">
   <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>